<commit_message>
change model unable to import form excel for date
</commit_message>
<xml_diff>
--- a/hakguan_db.xlsx
+++ b/hakguan_db.xlsx
@@ -5,21 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\django_gegche\dproject01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\django_gegche\dproject01\POSLUN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="5630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="5630" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="시트1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="222">
   <si>
     <t>행사 성격</t>
   </si>
@@ -733,15 +735,226 @@
     <t>공모전</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>행사제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시작시간</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>끝시간</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강연자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>게임빌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>컴투스</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설명회</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>채용설명회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임빌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>학생회관</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>층</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로비</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제12회 일월문화제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포스텍 문화 프로그램</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토의회 기념품점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일원문화제 흥!망!성!쇠!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학생회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일월문화제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클래식 기타 앙상블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입학처장님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;\ am/pm\ h:mm"/>
+    <numFmt numFmtId="180" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -777,6 +990,26 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -798,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -822,11 +1055,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1600,10 +1874,10 @@
       <c r="F17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="20" t="s">
         <v>98</v>
       </c>
       <c r="I17" s="3"/>
@@ -1624,8 +1898,8 @@
       <c r="F18" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1644,8 +1918,8 @@
       <c r="F19" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1667,7 +1941,7 @@
       <c r="G20" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="3"/>
       <c r="J20" s="6" t="s">
         <v>109</v>
@@ -1691,7 +1965,7 @@
       <c r="G21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1713,7 +1987,7 @@
       <c r="G22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="3"/>
       <c r="J22" s="6" t="s">
         <v>109</v>
@@ -1734,10 +2008,10 @@
       <c r="F23" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1756,8 +2030,8 @@
       <c r="F24" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1776,8 +2050,8 @@
       <c r="F25" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1796,8 +2070,8 @@
       <c r="F26" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1816,8 +2090,8 @@
       <c r="F27" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1836,8 +2110,8 @@
       <c r="F28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1856,8 +2130,8 @@
       <c r="F29" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1879,7 +2153,7 @@
       <c r="G30" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="9"/>
+      <c r="H30" s="21"/>
       <c r="I30" s="3"/>
       <c r="J30" s="6" t="s">
         <v>109</v>
@@ -1928,10 +2202,10 @@
       <c r="F32" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="20" t="s">
         <v>149</v>
       </c>
       <c r="I32" s="3"/>
@@ -1954,8 +2228,8 @@
       <c r="F33" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
       <c r="I33" s="3"/>
       <c r="J33" s="6" t="s">
         <v>154</v>
@@ -2000,10 +2274,10 @@
       <c r="F35" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="20" t="s">
         <v>164</v>
       </c>
       <c r="I35" s="3"/>
@@ -2024,8 +2298,8 @@
       <c r="F36" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
       <c r="I36" s="3"/>
       <c r="J36" s="4"/>
       <c r="K36" s="3"/>
@@ -2044,8 +2318,8 @@
       <c r="F37" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
       <c r="I37" s="3"/>
       <c r="J37" s="4"/>
       <c r="K37" s="3"/>
@@ -2064,8 +2338,8 @@
       <c r="F38" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
       <c r="I38" s="3"/>
       <c r="J38" s="4"/>
       <c r="K38" s="3"/>
@@ -2084,8 +2358,8 @@
       <c r="F39" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
       <c r="I39" s="3"/>
       <c r="J39" s="4"/>
       <c r="K39" s="3"/>
@@ -2104,8 +2378,8 @@
       <c r="F40" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
       <c r="I40" s="3"/>
       <c r="J40" s="4"/>
       <c r="K40" s="3"/>
@@ -2124,8 +2398,8 @@
       <c r="F41" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
       <c r="I41" s="3"/>
       <c r="J41" s="4"/>
       <c r="K41" s="3"/>
@@ -2144,8 +2418,8 @@
       <c r="F42" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
       <c r="K42" s="3"/>
@@ -2164,8 +2438,8 @@
       <c r="F43" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
       <c r="I43" s="3"/>
       <c r="J43" s="4"/>
       <c r="K43" s="3"/>
@@ -2184,8 +2458,8 @@
       <c r="F44" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
       <c r="I44" s="3"/>
       <c r="J44" s="4"/>
       <c r="K44" s="3"/>
@@ -2204,8 +2478,8 @@
       <c r="F45" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
       <c r="I45" s="3"/>
       <c r="J45" s="4"/>
       <c r="K45" s="3"/>
@@ -2231,7 +2505,7 @@
         <v>199</v>
       </c>
       <c r="I46" s="3"/>
-      <c r="J46" s="10" t="s">
+      <c r="J46" s="9" t="s">
         <v>200</v>
       </c>
       <c r="K46" s="3"/>
@@ -2887,4 +3161,352 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.90625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="18">
+        <v>171011</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1700</v>
+      </c>
+      <c r="D2" s="18">
+        <v>1900</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="19">
+        <v>171012</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1200</v>
+      </c>
+      <c r="D3" s="19">
+        <v>1300</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="19">
+        <v>170928</v>
+      </c>
+      <c r="C4" s="19">
+        <v>1220</v>
+      </c>
+      <c r="D4" s="19">
+        <v>1320</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" s="19">
+        <v>171020</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1700</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2100</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A6" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="19">
+        <v>171019</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1930</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2100</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.90625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="23">
+        <v>43054</v>
+      </c>
+      <c r="C1" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="22">
+        <v>43020</v>
+      </c>
+      <c r="C2" s="25">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="22">
+        <v>43006</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.625</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="22">
+        <v>43028</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="22">
+        <v>43027</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A6" s="13"/>
+      <c r="B6" s="24"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="A7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>